<commit_message>
Corrige error en archivo
</commit_message>
<xml_diff>
--- a/tests/data/datos_pruebas_sin_errores/IG_POSICION_TRAMPAS_14JUN2020.xlsx
+++ b/tests/data/datos_pruebas_sin_errores/IG_POSICION_TRAMPAS_14JUN2020.xlsx
@@ -5571,10 +5571,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1641" activeCellId="0" sqref="A1641"/>
+      <selection pane="bottomLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
@@ -19961,7 +19961,7 @@
         <v>16</v>
       </c>
       <c r="H411" s="10" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="I411" s="10" t="s">
         <v>16</v>
@@ -63091,7 +63091,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">

</xml_diff>